<commit_message>
add buttons for Indicators and Parameters
add "add buttons"
</commit_message>
<xml_diff>
--- a/src/main/webapp/images/images.xlsx
+++ b/src/main/webapp/images/images.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao\Documents\git\GoalArch\src\main\webapp\images\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C77ACB4-65B0-4926-A08B-94479635D8D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="7635" windowHeight="4680"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -14,8 +20,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +65,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -66,25 +80,31 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>281263</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46983</xdr:rowOff>
+      <xdr:rowOff>92966</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>523874</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>74542</xdr:rowOff>
+      <xdr:rowOff>120525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Retângulo de cantos arredondados 1"/>
+        <xdr:cNvPr id="2" name="Retângulo de cantos arredondados 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2120002" y="237483"/>
+          <a:off x="1503091" y="283466"/>
           <a:ext cx="242611" cy="218059"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -131,202 +151,31 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>119339</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>113658</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>132461</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109245</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>319363</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>123183</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>375072</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>136804</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Retângulo de cantos arredondados 4"/>
+        <xdr:cNvPr id="7" name="Retângulo de cantos arredondados 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2557739" y="1066158"/>
-          <a:ext cx="200024" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" b="1">
-              <a:latin typeface="Arial Black" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>-</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>52664</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>18408</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>252688</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>27933</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Retângulo de cantos arredondados 3"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2491064" y="208908"/>
-          <a:ext cx="200024" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" b="1">
-              <a:latin typeface="Arial Black" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>T</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>386039</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>8883</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>586063</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>18408</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Retângulo de cantos arredondados 5"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2824439" y="199383"/>
-          <a:ext cx="200024" cy="200025"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent6">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" b="1">
-              <a:latin typeface="Arial Black" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Q</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>355806</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>30418</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>598417</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>57977</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Retângulo de cantos arredondados 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2194545" y="792418"/>
+          <a:off x="1965202" y="299745"/>
           <a:ext cx="242611" cy="218059"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -373,25 +222,31 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>107328</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>63549</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>600001</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109532</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>349939</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>91108</xdr:rowOff>
+      <xdr:colOff>231698</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>137091</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Retângulo de cantos arredondados 7"/>
+        <xdr:cNvPr id="8" name="Retângulo de cantos arredondados 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2558980" y="635049"/>
+          <a:off x="2432742" y="300032"/>
           <a:ext cx="242611" cy="218059"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -438,25 +293,31 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>364089</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>154657</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>442916</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>102105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>606700</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>182216</xdr:rowOff>
+      <xdr:colOff>74613</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>129664</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Retângulo de cantos arredondados 8"/>
+        <xdr:cNvPr id="9" name="Retângulo de cantos arredondados 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3428654" y="726157"/>
+          <a:off x="2886571" y="292605"/>
           <a:ext cx="242611" cy="218059"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -499,13 +360,185 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>289034</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>531645</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>53835</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Retângulo de cantos arredondados 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7043AD11-2598-4F05-8D30-E8A0B72539D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1510862" y="788276"/>
+          <a:ext cx="242611" cy="218059"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>+</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>I</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>34158</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>14452</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>276769</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>42011</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Retângulo de cantos arredondados 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{829C69E5-39D4-4E7A-987B-5D381BE03F4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866899" y="776452"/>
+          <a:ext cx="242611" cy="218059"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>+</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>P</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -543,9 +576,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -577,9 +610,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -611,9 +662,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -786,21 +855,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="13" width="9.140625" style="1"/>
     <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="17" ht="105.75" customHeight="1"/>
+    <row r="17" ht="105.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>